<commit_message>
v0.30 - Fix Interview
</commit_message>
<xml_diff>
--- a/static/Design_Template.xlsx
+++ b/static/Design_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\SnowBall\paper_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\SnowBall\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5298334-23EB-41D7-B73F-0FA767226361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991B232E-8A7E-4ED4-9340-09E11F100BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28845" yWindow="16080" windowWidth="29040" windowHeight="15720" tabRatio="873" firstSheet="2" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="873" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RCM" sheetId="1" r:id="rId1"/>
@@ -26,23 +26,25 @@
     <sheet name="APD10" sheetId="11" r:id="rId11"/>
     <sheet name="APD11" sheetId="12" r:id="rId12"/>
     <sheet name="APD12" sheetId="13" r:id="rId13"/>
-    <sheet name="PC01" sheetId="14" r:id="rId14"/>
-    <sheet name="PC02" sheetId="15" r:id="rId15"/>
-    <sheet name="PC03" sheetId="16" r:id="rId16"/>
-    <sheet name="PC04" sheetId="17" r:id="rId17"/>
-    <sheet name="PC05" sheetId="18" r:id="rId18"/>
-    <sheet name="CO01" sheetId="19" r:id="rId19"/>
-    <sheet name="CO02" sheetId="20" r:id="rId20"/>
-    <sheet name="CO03" sheetId="21" r:id="rId21"/>
-    <sheet name="CO04" sheetId="22" r:id="rId22"/>
-    <sheet name="CO05" sheetId="23" r:id="rId23"/>
-    <sheet name="CO06" sheetId="24" r:id="rId24"/>
+    <sheet name="APD13" sheetId="25" r:id="rId14"/>
+    <sheet name="APD14" sheetId="26" r:id="rId15"/>
+    <sheet name="PC01" sheetId="14" r:id="rId16"/>
+    <sheet name="PC02" sheetId="15" r:id="rId17"/>
+    <sheet name="PC03" sheetId="16" r:id="rId18"/>
+    <sheet name="PC04" sheetId="17" r:id="rId19"/>
+    <sheet name="PC05" sheetId="18" r:id="rId20"/>
+    <sheet name="CO01" sheetId="19" r:id="rId21"/>
+    <sheet name="CO02" sheetId="20" r:id="rId22"/>
+    <sheet name="CO03" sheetId="21" r:id="rId23"/>
+    <sheet name="CO04" sheetId="22" r:id="rId24"/>
+    <sheet name="CO05" sheetId="23" r:id="rId25"/>
+    <sheet name="CO06" sheetId="24" r:id="rId26"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId25"/>
-    <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
     <externalReference r:id="rId28"/>
+    <externalReference r:id="rId29"/>
+    <externalReference r:id="rId30"/>
   </externalReferences>
   <definedNames>
     <definedName name="_1.매출채권">#REF!</definedName>
@@ -88,17 +90,19 @@
     <definedName name="_xlnm.Print_Area" localSheetId="10">'APD10'!$A$1:$C$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'APD11'!$A$1:$C$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">'APD12'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="18">'CO01'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="19">'CO02'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="20">'CO03'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="21">'CO04'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="22">'CO05'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="23">'CO06'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="13">'PC01'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="14">'PC02'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="15">'PC03'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="16">'PC04'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="17">'PC05'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="13">'APD13'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="14">'APD14'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="20">'CO01'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="21">'CO02'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="22">'CO03'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="23">'CO04'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="24">'CO05'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="25">'CO06'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="15">'PC01'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="16">'PC02'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="17">'PC03'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="18">'PC04'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="19">'PC05'!$A$1:$C$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">RCM!$A$1:$E$46</definedName>
     <definedName name="_xlnm.Print_Area">#REF!</definedName>
     <definedName name="Print_Area_MI">#REF!</definedName>
@@ -127,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="118">
   <si>
     <t>Client</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -1631,9 +1635,9 @@
   <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B9" sqref="B9:C10"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -3548,6 +3552,392 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A361A614-467E-4805-85AC-D8607985F816}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="134.1640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" style="11" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A1" s="18"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" ht="32.25" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="15"/>
+      <c r="B11" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="33"/>
+    </row>
+    <row r="13" spans="1:4" ht="300" customHeight="1">
+      <c r="A13" s="9"/>
+      <c r="B13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="33"/>
+    </row>
+    <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="15"/>
+      <c r="B14" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="36"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1">
+      <c r="A15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1">
+      <c r="B16" s="13"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="2:4" ht="15" customHeight="1">
+      <c r="B17" s="13"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="2:4" ht="15" customHeight="1">
+      <c r="B18" s="13"/>
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="2:4" ht="15" customHeight="1">
+      <c r="B19" s="13"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="2:4" ht="15" customHeight="1">
+      <c r="B20" s="13"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="2:4" ht="15" customHeight="1">
+      <c r="B21" s="13"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="2:4" ht="15" customHeight="1">
+      <c r="B22" s="13"/>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="2:4" ht="15" customHeight="1">
+      <c r="B23" s="13"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="2:4" ht="15" customHeight="1">
+      <c r="B24" s="13"/>
+      <c r="D24" s="19"/>
+    </row>
+    <row r="25" spans="2:4" ht="15" customHeight="1">
+      <c r="B25" s="13"/>
+      <c r="D25" s="19"/>
+    </row>
+    <row r="26" spans="2:4" ht="15" customHeight="1">
+      <c r="B26" s="13"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="2:4" ht="15" customHeight="1">
+      <c r="B27" s="13"/>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="2:4" ht="15" customHeight="1">
+      <c r="B28" s="13"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="2:4" ht="15" customHeight="1">
+      <c r="B29" s="13"/>
+      <c r="D29" s="19"/>
+    </row>
+    <row r="30" spans="2:4" ht="15" customHeight="1">
+      <c r="B30" s="13"/>
+      <c r="D30" s="19"/>
+    </row>
+    <row r="31" spans="2:4" ht="15" customHeight="1">
+      <c r="B31" s="13"/>
+      <c r="D31" s="19"/>
+    </row>
+    <row r="32" spans="2:4" ht="15" customHeight="1">
+      <c r="B32" s="13"/>
+      <c r="D32" s="19"/>
+    </row>
+    <row r="33" spans="4:4" ht="15" customHeight="1">
+      <c r="D33" s="19"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.70866141732283472" bottom="0" header="0.51181102362204722" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" scale="53" fitToHeight="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40AF2F6-052D-44E3-ABE0-B0ABDF723B15}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="134.1640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" style="11" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A1" s="18"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" ht="32.25" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="15"/>
+      <c r="B11" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="33"/>
+    </row>
+    <row r="13" spans="1:4" ht="300" customHeight="1">
+      <c r="A13" s="9"/>
+      <c r="B13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="33"/>
+    </row>
+    <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="15"/>
+      <c r="B14" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="36"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1">
+      <c r="A15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1">
+      <c r="B16" s="13"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="2:4" ht="15" customHeight="1">
+      <c r="B17" s="13"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="2:4" ht="15" customHeight="1">
+      <c r="B18" s="13"/>
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="2:4" ht="15" customHeight="1">
+      <c r="B19" s="13"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="2:4" ht="15" customHeight="1">
+      <c r="B20" s="13"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="2:4" ht="15" customHeight="1">
+      <c r="B21" s="13"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="2:4" ht="15" customHeight="1">
+      <c r="B22" s="13"/>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="2:4" ht="15" customHeight="1">
+      <c r="B23" s="13"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="2:4" ht="15" customHeight="1">
+      <c r="B24" s="13"/>
+      <c r="D24" s="19"/>
+    </row>
+    <row r="25" spans="2:4" ht="15" customHeight="1">
+      <c r="B25" s="13"/>
+      <c r="D25" s="19"/>
+    </row>
+    <row r="26" spans="2:4" ht="15" customHeight="1">
+      <c r="B26" s="13"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="2:4" ht="15" customHeight="1">
+      <c r="B27" s="13"/>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="2:4" ht="15" customHeight="1">
+      <c r="B28" s="13"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="2:4" ht="15" customHeight="1">
+      <c r="B29" s="13"/>
+      <c r="D29" s="19"/>
+    </row>
+    <row r="30" spans="2:4" ht="15" customHeight="1">
+      <c r="B30" s="13"/>
+      <c r="D30" s="19"/>
+    </row>
+    <row r="31" spans="2:4" ht="15" customHeight="1">
+      <c r="B31" s="13"/>
+      <c r="D31" s="19"/>
+    </row>
+    <row r="32" spans="2:4" ht="15" customHeight="1">
+      <c r="B32" s="13"/>
+      <c r="D32" s="19"/>
+    </row>
+    <row r="33" spans="4:4" ht="15" customHeight="1">
+      <c r="D33" s="19"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.70866141732283472" bottom="0" header="0.51181102362204722" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" scale="53" fitToHeight="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892276DF-69D8-4934-A2D1-779B59881CC6}">
   <dimension ref="A1:D33"/>
   <sheetViews>
@@ -3740,7 +4130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780BC2CA-A325-48E0-AF2E-909F71B1AF19}">
   <dimension ref="A1:D33"/>
   <sheetViews>
@@ -3933,7 +4323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F848FF76-7E7F-4F50-B88A-661EF1A1990E}">
   <dimension ref="A1:D33"/>
   <sheetViews>
@@ -4126,394 +4516,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74176A7-CD9C-4F01-AB7C-84BDA9AF8B37}">
-  <dimension ref="A1:D33"/>
-  <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="134.1640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.6640625" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A1" s="18"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="17"/>
-    </row>
-    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="29.25" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:4" ht="32.25" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="32"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="33"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="34"/>
-    </row>
-    <row r="11" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="33"/>
-    </row>
-    <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="33"/>
-    </row>
-    <row r="13" spans="1:4" ht="300" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="33"/>
-    </row>
-    <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="36"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="20"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1">
-      <c r="B16" s="13"/>
-      <c r="D16" s="19"/>
-    </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
-      <c r="B17" s="13"/>
-      <c r="D17" s="19"/>
-    </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
-      <c r="B18" s="13"/>
-      <c r="D18" s="19"/>
-    </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
-      <c r="B19" s="13"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
-      <c r="B20" s="13"/>
-      <c r="D20" s="19"/>
-    </row>
-    <row r="21" spans="2:4" ht="15" customHeight="1">
-      <c r="B21" s="13"/>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="2:4" ht="15" customHeight="1">
-      <c r="B22" s="13"/>
-      <c r="D22" s="19"/>
-    </row>
-    <row r="23" spans="2:4" ht="15" customHeight="1">
-      <c r="B23" s="13"/>
-      <c r="D23" s="19"/>
-    </row>
-    <row r="24" spans="2:4" ht="15" customHeight="1">
-      <c r="B24" s="13"/>
-      <c r="D24" s="19"/>
-    </row>
-    <row r="25" spans="2:4" ht="15" customHeight="1">
-      <c r="B25" s="13"/>
-      <c r="D25" s="19"/>
-    </row>
-    <row r="26" spans="2:4" ht="15" customHeight="1">
-      <c r="B26" s="13"/>
-      <c r="D26" s="19"/>
-    </row>
-    <row r="27" spans="2:4" ht="15" customHeight="1">
-      <c r="B27" s="13"/>
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="2:4" ht="15" customHeight="1">
-      <c r="B28" s="13"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="2:4" ht="15" customHeight="1">
-      <c r="B29" s="13"/>
-      <c r="D29" s="19"/>
-    </row>
-    <row r="30" spans="2:4" ht="15" customHeight="1">
-      <c r="B30" s="13"/>
-      <c r="D30" s="19"/>
-    </row>
-    <row r="31" spans="2:4" ht="15" customHeight="1">
-      <c r="B31" s="13"/>
-      <c r="D31" s="19"/>
-    </row>
-    <row r="32" spans="2:4" ht="15" customHeight="1">
-      <c r="B32" s="13"/>
-      <c r="D32" s="19"/>
-    </row>
-    <row r="33" spans="4:4" ht="15" customHeight="1">
-      <c r="D33" s="19"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.70866141732283472" bottom="0" header="0.51181102362204722" footer="0.11811023622047245"/>
-  <pageSetup paperSize="9" scale="53" fitToHeight="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF1AE05-26E5-4BB3-97EC-337AAEED2B82}">
-  <dimension ref="A1:D33"/>
-  <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="134.1640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.6640625" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A1" s="18"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="17"/>
-    </row>
-    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="29.25" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:4" ht="32.25" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="32"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="33"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="34"/>
-    </row>
-    <row r="11" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="33"/>
-    </row>
-    <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="33"/>
-    </row>
-    <row r="13" spans="1:4" ht="300" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="33"/>
-    </row>
-    <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="36"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="20"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1">
-      <c r="B16" s="13"/>
-      <c r="D16" s="19"/>
-    </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
-      <c r="B17" s="13"/>
-      <c r="D17" s="19"/>
-    </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
-      <c r="B18" s="13"/>
-      <c r="D18" s="19"/>
-    </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1">
-      <c r="B19" s="13"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1">
-      <c r="B20" s="13"/>
-      <c r="D20" s="19"/>
-    </row>
-    <row r="21" spans="2:4" ht="15" customHeight="1">
-      <c r="B21" s="13"/>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="2:4" ht="15" customHeight="1">
-      <c r="B22" s="13"/>
-      <c r="D22" s="19"/>
-    </row>
-    <row r="23" spans="2:4" ht="15" customHeight="1">
-      <c r="B23" s="13"/>
-      <c r="D23" s="19"/>
-    </row>
-    <row r="24" spans="2:4" ht="15" customHeight="1">
-      <c r="B24" s="13"/>
-      <c r="D24" s="19"/>
-    </row>
-    <row r="25" spans="2:4" ht="15" customHeight="1">
-      <c r="B25" s="13"/>
-      <c r="D25" s="19"/>
-    </row>
-    <row r="26" spans="2:4" ht="15" customHeight="1">
-      <c r="B26" s="13"/>
-      <c r="D26" s="19"/>
-    </row>
-    <row r="27" spans="2:4" ht="15" customHeight="1">
-      <c r="B27" s="13"/>
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="2:4" ht="15" customHeight="1">
-      <c r="B28" s="13"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="2:4" ht="15" customHeight="1">
-      <c r="B29" s="13"/>
-      <c r="D29" s="19"/>
-    </row>
-    <row r="30" spans="2:4" ht="15" customHeight="1">
-      <c r="B30" s="13"/>
-      <c r="D30" s="19"/>
-    </row>
-    <row r="31" spans="2:4" ht="15" customHeight="1">
-      <c r="B31" s="13"/>
-      <c r="D31" s="19"/>
-    </row>
-    <row r="32" spans="2:4" ht="15" customHeight="1">
-      <c r="B32" s="13"/>
-      <c r="D32" s="19"/>
-    </row>
-    <row r="33" spans="4:4" ht="15" customHeight="1">
-      <c r="D33" s="19"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.70866141732283472" bottom="0" header="0.51181102362204722" footer="0.11811023622047245"/>
-  <pageSetup paperSize="9" scale="53" fitToHeight="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27556D1-C6E7-4684-875A-7D2A6A33D8AB}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
@@ -4900,6 +4904,392 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF1AE05-26E5-4BB3-97EC-337AAEED2B82}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="134.1640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" style="11" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A1" s="18"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" ht="32.25" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="15"/>
+      <c r="B11" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="33"/>
+    </row>
+    <row r="13" spans="1:4" ht="300" customHeight="1">
+      <c r="A13" s="9"/>
+      <c r="B13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="33"/>
+    </row>
+    <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="15"/>
+      <c r="B14" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="36"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1">
+      <c r="A15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1">
+      <c r="B16" s="13"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="2:4" ht="15" customHeight="1">
+      <c r="B17" s="13"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="2:4" ht="15" customHeight="1">
+      <c r="B18" s="13"/>
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="2:4" ht="15" customHeight="1">
+      <c r="B19" s="13"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="2:4" ht="15" customHeight="1">
+      <c r="B20" s="13"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="2:4" ht="15" customHeight="1">
+      <c r="B21" s="13"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="2:4" ht="15" customHeight="1">
+      <c r="B22" s="13"/>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="2:4" ht="15" customHeight="1">
+      <c r="B23" s="13"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="2:4" ht="15" customHeight="1">
+      <c r="B24" s="13"/>
+      <c r="D24" s="19"/>
+    </row>
+    <row r="25" spans="2:4" ht="15" customHeight="1">
+      <c r="B25" s="13"/>
+      <c r="D25" s="19"/>
+    </row>
+    <row r="26" spans="2:4" ht="15" customHeight="1">
+      <c r="B26" s="13"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="2:4" ht="15" customHeight="1">
+      <c r="B27" s="13"/>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="2:4" ht="15" customHeight="1">
+      <c r="B28" s="13"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="2:4" ht="15" customHeight="1">
+      <c r="B29" s="13"/>
+      <c r="D29" s="19"/>
+    </row>
+    <row r="30" spans="2:4" ht="15" customHeight="1">
+      <c r="B30" s="13"/>
+      <c r="D30" s="19"/>
+    </row>
+    <row r="31" spans="2:4" ht="15" customHeight="1">
+      <c r="B31" s="13"/>
+      <c r="D31" s="19"/>
+    </row>
+    <row r="32" spans="2:4" ht="15" customHeight="1">
+      <c r="B32" s="13"/>
+      <c r="D32" s="19"/>
+    </row>
+    <row r="33" spans="4:4" ht="15" customHeight="1">
+      <c r="D33" s="19"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.70866141732283472" bottom="0" header="0.51181102362204722" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" scale="53" fitToHeight="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27556D1-C6E7-4684-875A-7D2A6A33D8AB}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="134.1640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" style="11" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A1" s="18"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" ht="32.25" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="15"/>
+      <c r="B11" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="33"/>
+    </row>
+    <row r="13" spans="1:4" ht="300" customHeight="1">
+      <c r="A13" s="9"/>
+      <c r="B13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="33"/>
+    </row>
+    <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="15"/>
+      <c r="B14" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="36"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1">
+      <c r="A15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1">
+      <c r="B16" s="13"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="2:4" ht="15" customHeight="1">
+      <c r="B17" s="13"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="2:4" ht="15" customHeight="1">
+      <c r="B18" s="13"/>
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="2:4" ht="15" customHeight="1">
+      <c r="B19" s="13"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="2:4" ht="15" customHeight="1">
+      <c r="B20" s="13"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="2:4" ht="15" customHeight="1">
+      <c r="B21" s="13"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="2:4" ht="15" customHeight="1">
+      <c r="B22" s="13"/>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="2:4" ht="15" customHeight="1">
+      <c r="B23" s="13"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="2:4" ht="15" customHeight="1">
+      <c r="B24" s="13"/>
+      <c r="D24" s="19"/>
+    </row>
+    <row r="25" spans="2:4" ht="15" customHeight="1">
+      <c r="B25" s="13"/>
+      <c r="D25" s="19"/>
+    </row>
+    <row r="26" spans="2:4" ht="15" customHeight="1">
+      <c r="B26" s="13"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="2:4" ht="15" customHeight="1">
+      <c r="B27" s="13"/>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="2:4" ht="15" customHeight="1">
+      <c r="B28" s="13"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="2:4" ht="15" customHeight="1">
+      <c r="B29" s="13"/>
+      <c r="D29" s="19"/>
+    </row>
+    <row r="30" spans="2:4" ht="15" customHeight="1">
+      <c r="B30" s="13"/>
+      <c r="D30" s="19"/>
+    </row>
+    <row r="31" spans="2:4" ht="15" customHeight="1">
+      <c r="B31" s="13"/>
+      <c r="D31" s="19"/>
+    </row>
+    <row r="32" spans="2:4" ht="15" customHeight="1">
+      <c r="B32" s="13"/>
+      <c r="D32" s="19"/>
+    </row>
+    <row r="33" spans="4:4" ht="15" customHeight="1">
+      <c r="D33" s="19"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.70866141732283472" bottom="0" header="0.51181102362204722" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" scale="53" fitToHeight="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67FB3B9-D9AE-4A28-B0F2-8C8615D161F7}">
   <dimension ref="A1:D33"/>
   <sheetViews>
@@ -5092,7 +5482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EEF343-0158-43A8-AEF9-6F1BCEDBEB8D}">
   <dimension ref="A1:D33"/>
   <sheetViews>
@@ -5285,7 +5675,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7177D00F-B1E7-446F-BD85-D04C922046B4}">
   <dimension ref="A1:D33"/>
   <sheetViews>
@@ -5478,7 +5868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9121B72A-A365-4A08-9925-1D2F2C9A6325}">
   <dimension ref="A1:D33"/>
   <sheetViews>
@@ -5671,11 +6061,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A05267E-DD4E-46E4-9CE0-1BF9CCF95E6E}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -7216,6 +7606,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x010100339A91ABF6B0E74BBAB45B3A7F6E62EE" ma:contentTypeVersion="" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="6e17012235b26a7a0350590f144b58ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1bbecb3f91f6338ad1582cc9b6c688ac" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7347,25 +7755,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC26BC8C-8D44-46BE-A39D-C16F3FC5094C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9F50EA-511A-47A0-93D9-E0B615D1BBD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4667855A-3738-433F-9E1F-E8508E1FE58D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7381,22 +7789,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9F50EA-511A-47A0-93D9-E0B615D1BBD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC26BC8C-8D44-46BE-A39D-C16F3FC5094C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
v0.33 - Add AI Reivew
</commit_message>
<xml_diff>
--- a/static/Design_Template.xlsx
+++ b/static/Design_Template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newsistraphael/Pythons/SnowBall/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\snowball\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD87C3-8F7A-1648-AF4E-BFFC1189D415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8CD8C0-B1EA-47D1-9129-879C3B9E65A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" tabRatio="873" firstSheet="10" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28845" yWindow="16080" windowWidth="29040" windowHeight="15720" tabRatio="873" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RCM" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="APD01" sheetId="2" r:id="rId2"/>
     <sheet name="APD02" sheetId="3" r:id="rId3"/>
     <sheet name="APD03" sheetId="4" r:id="rId4"/>
@@ -23,11 +23,11 @@
     <sheet name="APD07" sheetId="8" r:id="rId8"/>
     <sheet name="APD08" sheetId="9" r:id="rId9"/>
     <sheet name="APD09" sheetId="10" r:id="rId10"/>
-    <sheet name="APD10" sheetId="11" r:id="rId11"/>
-    <sheet name="APD11" sheetId="12" r:id="rId12"/>
+    <sheet name="APD10" sheetId="12" r:id="rId11"/>
+    <sheet name="APD11" sheetId="11" r:id="rId12"/>
     <sheet name="APD12" sheetId="13" r:id="rId13"/>
-    <sheet name="APD13" sheetId="25" r:id="rId14"/>
-    <sheet name="APD14" sheetId="26" r:id="rId15"/>
+    <sheet name="APD13" sheetId="26" r:id="rId14"/>
+    <sheet name="APD14" sheetId="25" r:id="rId15"/>
     <sheet name="PC01" sheetId="14" r:id="rId16"/>
     <sheet name="PC02" sheetId="15" r:id="rId17"/>
     <sheet name="PC03" sheetId="16" r:id="rId18"/>
@@ -49,10 +49,6 @@
   <definedNames>
     <definedName name="_1.매출채권">#REF!</definedName>
     <definedName name="※매출매트릭스">#REF!</definedName>
-    <definedName name="계">#REF!</definedName>
-    <definedName name="ㅁ1">#REF!</definedName>
-    <definedName name="진주원">'[2]4b Consolidated PL'!#REF!</definedName>
-    <definedName name="채권">#REF!</definedName>
     <definedName name="A">'[1]4b Consolidated PL'!#REF!</definedName>
     <definedName name="ddd">#REF!</definedName>
     <definedName name="LYN">'[2]4b Consolidated PL'!#REF!</definedName>
@@ -107,11 +103,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="17">'PC03'!$A$1:$C$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="18">'PC04'!$A$1:$C$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="19">'PC05'!$A$1:$C$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">RCM!$A$1:$E$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$A$1:$E$44</definedName>
     <definedName name="_xlnm.Print_Area">#REF!</definedName>
     <definedName name="Print_Area_MI">#REF!</definedName>
     <definedName name="Question_Type">[4]Values!$B$3:$B$10</definedName>
     <definedName name="SQL_Col">#REF!</definedName>
+    <definedName name="계">#REF!</definedName>
+    <definedName name="ㅁ1">#REF!</definedName>
+    <definedName name="진주원">'[2]4b Consolidated PL'!#REF!</definedName>
+    <definedName name="채권">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="100">
   <si>
     <t>Client</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -177,18 +177,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>주기</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>구분</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>테스트 절차</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
     <t>APD01</t>
   </si>
   <si>
@@ -246,12 +234,6 @@
     <t>PC05</t>
   </si>
   <si>
-    <t>PC06</t>
-  </si>
-  <si>
-    <t>PC07</t>
-  </si>
-  <si>
     <t>CO01</t>
   </si>
   <si>
@@ -309,21 +291,9 @@
     <t>DB 접근권한 승인</t>
   </si>
   <si>
-    <t>DB 패스워드</t>
-  </si>
-  <si>
-    <t>DB 관리자 권한 제한</t>
-  </si>
-  <si>
     <t>OS 접근권한 승인</t>
   </si>
   <si>
-    <t>OS 패스워드</t>
-  </si>
-  <si>
-    <t>OS 관리자 권한 제한</t>
-  </si>
-  <si>
     <t>프로그램 변경 승인</t>
   </si>
   <si>
@@ -333,18 +303,6 @@
     <t>프로그램 이관 승인</t>
   </si>
   <si>
-    <t>개발/운영 환경 분리</t>
-  </si>
-  <si>
-    <t>이관담당자 권한 제한</t>
-  </si>
-  <si>
-    <t>인프라 설정변경_DB</t>
-  </si>
-  <si>
-    <t>인프라 설정변경_OS</t>
-  </si>
-  <si>
     <t>배치잡 스케줄 등록 승인</t>
   </si>
   <si>
@@ -379,232 +337,12 @@
   </si>
   <si>
     <t>검수보고서 승인</t>
-  </si>
-  <si>
-    <t>Other</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quarterly</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Evently</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Daily</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>수동</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>자동</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>검토 결과</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>시스템그룹에서 작성하는 월간운영 현황 보고 문서에 백업 및 소산 내역의 작성 여부와 승인 여부를 검토한다
- 1. 모집단에서 샘플을 추출한다
- 2. 추출된 샘플의 백업 및 소산 결과가 정책서에 명시된 내용과 일치하는지 확인한다
- 3. 월간운영 현황 보고의 시스템 그룹장 승인 여부를 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>장애대응/재해복구 모의훈련은 평가 대상 기간 중 수행된 모의훈련 계획서 및 결과서 내용을 검토한다
- 1. 장애대응/재해복구 모의훈련 결과서가 적절한 승인권자의 승인을 득하였는지 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>패스워드 설정 내역을 검토하여 정책서와 상이한 부분이 존재하는지 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>데이터 센터 출입 통제 테스트는 아래와 같다
- 1. 출입 시스템에 등록된 출입 인가자 List의 적절성(서버담당자 직무를 보유한 인원)을 확인한다
- 2. 인가에 대한 승인 이력을 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>신규 권한 부여 시 권한 요청서 작성/승인 완료 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다.
-  2. 추출된 샘플의 권한 요청서 작성 여부와 부서장 승인 여부를 확인한다.
-  3. 권한 요청 및 승인 완료 후 권한 부여가 수행되었는지 확인한다
-    - 권한 요청서 작성/승인 일자 &lt; 권한부여 일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB 접근권한 요청서/승인 완료 여부를 검토한다.
-  1. 모집단에서 샘플을 추출한다.
-  2. 신규 부여된 권한(계정)에 대해 요청서 작성 여부와 승인 여부를 확인한다
-  3. 요청서 작성/승인 완료 후 계정 생성이 수행되었는지 확인한다
-    - 요청/승인 일자 &lt; 접근권한 부여 일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OS 접근권한 요청서/승인 완료 여부를 검토한다.
-  1. 모집단에서 샘플을 추출한다.
-  2. 신규 부여된 권한(계정)에 대해 요청서 작성 여부와 승인 여부를 확인한다
-  3. 요청서 작성/승인 완료 후 계정 생성이 수행되었는지 확인한다
-    - 요청/승인 일자 &lt; 접근권한 부여 일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB Superuser 계정에 대한 접근 제어 설정사항을 검토한다
-  1. 접근제어 Tool에 Sys/System/SA 등 Superuser 계정으로 접속 가능한 인원을 확인한다.
-  2. 해당 인원의 직무상 적합성 여부를 확인한다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OS Superuser 계정에 대한 접근 제어 설정사항을 검토한다
-  1. 접근제어 Tool에 root/administrator 등 Superuser 계정으로 접속 가능한 인원을 확인한다.
-  2. 해당 인원의 직무상 적합성 여부를 확인한다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로그램 변경 시 변경 요청서 작성/승인 완료 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다.
-  2. 추출된 샘플의 변경요청서 작성 여부와 부서장 승인 여부를 확인한다.
-  3. 변경요청서 작성/승인 완료 후 이관이 수행되었는지 확인한다
-    - 변경 요청/승인 일자 &lt; 이관일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로그램 변경시 요청자에 의한 사용자 테스트 완료 여부를 검토한다.
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플의 사용자 테스트 결과서 작성 여부를 확인한다
-  3. 사용자 테스트 완료 후 이관이 수행되었는지 확인한다
-    - 사용자 테스트 일자 &lt; 이관 일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로그램 변경시 이관 요청서 작성/승인 완료 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플의 이관요청서 작성 여부 승인 여부를 확인한다
-  3. 이관 승인 완료 후 이관이 수행되었는지 확인한다
-    - 이관 요청 작성/승인 일자&lt;이관일자</t>
-    <phoneticPr fontId="29" type="noConversion"/>
-  </si>
-  <si>
-    <t>이관권한을 보유한 인원이 직무분리상 해당 권한을 보유하고 있어야 하는 인원인지 검토한다
-  1. 이관권한을 보유한 인원이 직무상 이관담당자인지 확인한다
-  2. 이관담당자가 지정되어 있지 않은 경우 각 변경건에 대해 개발담당자와 이관담당자를 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>개발과 운영 환경이 논리적으로 분리되어 있으며 운영 환경에서는 개발 불가 설정을 검토한다
-  1. 시스템이 개발, 운영으로 분리되어 있음을 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>데이터 변경 시 요청서 작성 및 부서장의 승인 완료 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플의 데이터 변경 요청서 작성 여부와 부서장 승인 여부를 확인한다
-  3. 변경 요청서 작성 및 승인 완료 후 데이터 변경이 수행되었는지 확인한다
-    - 변경요청서 작성/승인 일자 &lt; 데이터 변경 일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB 변경사항(Patch History)에 대해 계획서와 승인 이력의 존재 여부를 검토한다
-  1. 모집단(DB Patch 이력)에서 샘플을 추출한다
-  2. 샘플에 대해 정기PM 계획서 등 변경에 대한 승인 이력을 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OS 변경사항(Patch History)에 대해 계획서와 승인 이력의 존재 여부를 검토한다
-  1. 모집단(OS Patch 이력)에서 샘플을 추출한다
-  2. 샘플에 대해 정기PM 계획서 등 변경에 대한 승인 이력을 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>구축된 시스템의 타당검 검토 및 부서장 승인 이력의 존재 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플건의 타당성 검토 문서가 작성되었는지 확인한다
-  3. 타당성 검토 문서가 부서장의 승인을 득하였는지 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>구축된 시스템의 타당검 검토 및 부서장 승인 이력의 존재 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플건의 요구사항 정의서가 작성되었는지 확인한다
-  3. 요구사항 정의서 문서가 부서장의 승인을 득하였는지 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>시스템 구축 및 Open 시 테스트 시나리오/결과서 완료 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플건의 규모와 기능에 따라 테스트(단위테스트, CRP테스트, EP테스트, 통합테스트, 사용자인수테스트) 시나리오와 결과서의 작성 여부를 확인한다
-  3. 테스트 완료 후 시스템 Open 되었음을 확인한다
-    - 테스트 일자 &lt; 시스템 Open 일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>시스템 구축 및 Open 시 데이터 이관(DC&amp;M) 계획서 및 결과서의 작성과 승인권자의 승인 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플건의 데이터 이관 계획서 및 결과서의 작성과 승인권자의 승인 여부를 확인한다
-  3. 데이터 이관 결과서 승인 완료 후 시스템 Open 되었음을 확인한다
-    - 데이터 이관 승인 일자 &lt; 시스템 Open 일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>시스템 구축 및 사용자 교육 계획이 수립되고 부서장의 승인 완료 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플건의 사용자 교육 계획서를 확인한다
-  3. 교육 계획서의 부서장의 승인 여부를 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>시스템 구축 및 Open 시 검수보고서 작성/승인 완료 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플건의 검수보고서 작성/승인 완료 여부를 확인한다
-  3. 검수보고서 작성/승인 완료 후 시스템 Open 되었음을 확인한다
-    - 검수보고서 작성/승인 일자 &lt; 시스템 Open 일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Batch 등록(변경)시 등록(변경) 요청서 작성 및 승인 완료 여부를 검토한다
-  1. 모집단에서 샘플을 추출한다
-  2. 추출된 샘플건의 등록(변경) 요청서의 작성 여부 및 승인 여부를 확인한다
-  3. 등록(변경) 요청서 작성 및 승인 완료 후 Batch 등록(변경)이 수행되었음을 확인한다
-    - 요청/승인 일자 &lt; 등록 일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Batch 등록권한 보유자의 직무상 적절성과 수행중인 Batch Job의 등록자를 검토한다
-  1. Batch 등록 권한 보유자를 조회하여 직무상 적절한 인원(IT담당자 등)이 보유하고 있는지 확인한다
-  2. Batch 등록 권한이 현업에게 있는 경우 실제 등록된 Batch의 등록자를 대상으로 적정성 여부를 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Batch 오류건에 대해 원인 파악 및 조치 여부를 검토한다
-  1. 모집단(당기 Batch 오류 List)에서 샘플을 추출한다
-  2. 샘플에 대해 원인 파악 및 조치 여부가 문서화되어 있는지 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>데이터 변경 권한자의 적정성 여부를 검토한다
-  1. 데이터 변경 권한 보유자를 조회한다
-  2. 권한 보유자의 직무 등을 검토하여 적정한 인원이 권한을 보유하고 있는지 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Application 관리자 권한 보유자자의 적정성 여부를 검토한다
-  1. 관리자 권한 보유자를 조회한다
-  2. 권한 보유자의 직무 등을 검토하여 적정한 인원이 권한을 보유하고 있는지 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>부서이동자의 권한이 적시에 회수되었는지 검토한다
-  1. 모집단(당기 부서이동자)에서 샘플을 추출한다
-  2. 샘플에 선정된 인원이 부서 이동 전 보유하고 있는 권한이 모두 회수되었는지 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Application 퇴사자 접근 권한 회수</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -613,19 +351,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>퇴사자의 접근 권한이 적시에 회수되었는지 검토한다
-  1. 모집단(당기 퇴사자)에서 샘플을 추출한다
-  2. 샘플에 선정된 인원의 접근권한이 회수되었는지 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>당기 권한 Monitoring이 수행되고 승인권자의 승인이 완료되었는지 검토한다
-  1. 통제 주기에 따라 샘플을 선정한다
-  2. 샘플의 Monitoring 문서가 전체 권한을 대상으로 검토되었는지 확인한다
-  3. Monitoring 문서의 승인 여부를 확인한다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>당기 승인이력이 있는 권한신청서를 첨부하세요</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -716,6 +441,42 @@
   <si>
     <t>서버실 출입에 관련된 증빙을 첨부하세요</t>
     <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>결론</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>검토결과</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>개선필요사항</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>이관담당자 권한 제한</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발/운영 환경 분리</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB 관리자 권한 제한</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB 패스워드</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OS 관리자 권한 제한</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OS 패스워드</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -733,7 +494,7 @@
     <numFmt numFmtId="183" formatCode="hh:mm:ss"/>
     <numFmt numFmtId="184" formatCode="yyyy&quot;년&quot;\ m&quot;월&quot;\ d&quot;일&quot;;@"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <name val="돋움"/>
@@ -919,13 +680,6 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1219,20 +973,6 @@
     <cellStyle name="??&amp;O?&amp;H?_x0008__x000f__x0007_?_x0007__x0001__x0001_" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="??&amp;O?&amp;H?_x0008_??_x0007__x0001__x0001_" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="뒤에 오는 하이퍼링크_금융비용자본화" xfId="5" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="뷭?_BOOKSHIP" xfId="6" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="새귑_롤痰삠悧 " xfId="8" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="새귑[0]_롤痰삠悧 " xfId="7" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="스타일 1" xfId="1" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="지정되지 않음" xfId="9" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="콤마 [0]_  종  합  " xfId="10" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="콤마_  종  합  " xfId="11" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="표준 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="標準_Akia(F）-8" xfId="12" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="표준_Operating_test(1)" xfId="13" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="표준_Sheet1" xfId="14" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
     <cellStyle name="category" xfId="15" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Comma [0]_ SG&amp;A Bridge " xfId="16" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="comma zerodec" xfId="17" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
@@ -1257,6 +997,20 @@
     <cellStyle name="Output Report Title" xfId="35" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="Percent [2]" xfId="36" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
     <cellStyle name="subhead" xfId="37" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="뒤에 오는 하이퍼링크_금융비용자본화" xfId="5" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="뷭?_BOOKSHIP" xfId="6" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="새귑[0]_롤痰삠悧 " xfId="7" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="새귑_롤痰삠悧 " xfId="8" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="스타일 1" xfId="1" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="지정되지 않음" xfId="9" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="콤마 [0]_  종  합  " xfId="10" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="콤마_  종  합  " xfId="11" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="표준 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="標準_Akia(F）-8" xfId="12" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="표준_Operating_test(1)" xfId="13" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="표준_Sheet1" xfId="14" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1307,24 +1061,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="1 START HERE | Overview"/>
-      <sheetName val="2 Financial &amp; Disclosure Accts"/>
-      <sheetName val="3 Cycles &amp; Transactions"/>
-      <sheetName val="4 Transaction Risk Assessment"/>
-      <sheetName val="4c Cycle Coverage"/>
-      <sheetName val="4a Consolidated BS"/>
       <sheetName val="4b Consolidated PL"/>
-      <sheetName val=" Notes On Categories"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1334,46 +1074,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="결과 (2)"/>
-      <sheetName val="포항"/>
-      <sheetName val="TWB"/>
-      <sheetName val="결과"/>
       <sheetName val="SETUP"/>
-      <sheetName val="도움말"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4">
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>HQ</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>PP</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>KP</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>BP</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>%</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1739,20 +1443,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B9" sqref="B9:C10"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="109.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="23.6640625" customWidth="1"/>
   </cols>
@@ -1765,660 +1469,454 @@
         <v>10</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="B2" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="29"/>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="B3" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A4" s="31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="96">
-      <c r="A2" s="31" t="s">
+      <c r="B4" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="29"/>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B5" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A6" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="29"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A7" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A9" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A3" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A4" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A5" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="31" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A10" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="80">
-      <c r="A6" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="31" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A11" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A12" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A13" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="16">
-      <c r="A7" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="31" t="s">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A14" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A15" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A16" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="96">
-      <c r="A8" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="31" t="s">
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A17" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A9" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="31" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="29"/>
+    </row>
+    <row r="18" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A18" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="96">
-      <c r="A10" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="31" t="s">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="37"/>
+    </row>
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A19" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A20" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A21" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="16">
-      <c r="A11" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="31" t="s">
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A22" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A12" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="31" t="s">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A23" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" ht="96">
-      <c r="A13" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="31" t="s">
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A24" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" ht="16">
-      <c r="A14" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="31" t="s">
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="29"/>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A25" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A15" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="31" t="s">
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="29"/>
+    </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A26" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="3" customFormat="1" ht="96">
-      <c r="A16" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="31" t="s">
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="29"/>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A27" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" ht="96">
-      <c r="A17" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="31" t="s">
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="29"/>
+    </row>
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A28" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" ht="96">
-      <c r="A18" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="31" t="s">
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A29" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="48">
-      <c r="A19" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="31" t="s">
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="29"/>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A30" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A20" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="31" t="s">
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="29"/>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A31" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A21" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="31" t="s">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" ht="13.5">
+      <c r="A32" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A22" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" ht="96">
-      <c r="A23" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A24" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" ht="64">
-      <c r="A25" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="32">
-      <c r="A26" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" ht="80">
-      <c r="A27" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="48">
-      <c r="A28" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" ht="80">
-      <c r="A29" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="80">
-      <c r="A30" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="112">
-      <c r="A31" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" ht="96">
-      <c r="A32" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="80">
-      <c r="A33" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="96">
-      <c r="A34" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="29"/>
+    </row>
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+    </row>
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="27"/>
       <c r="B35" s="27"/>
       <c r="C35" s="28"/>
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="27"/>
       <c r="B36" s="27"/>
       <c r="C36" s="28"/>
       <c r="D36" s="29"/>
       <c r="E36" s="29"/>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="27"/>
       <c r="B37" s="27"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="27"/>
       <c r="B38" s="27"/>
       <c r="C38" s="28"/>
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="27"/>
       <c r="B39" s="27"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="27"/>
       <c r="B40" s="27"/>
       <c r="C40" s="28"/>
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="27"/>
       <c r="B41" s="27"/>
       <c r="C41" s="28"/>
       <c r="D41" s="29"/>
       <c r="E41" s="29"/>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="27"/>
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="43" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="27"/>
       <c r="B43" s="27"/>
       <c r="C43" s="28"/>
       <c r="D43" s="29"/>
       <c r="E43" s="29"/>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="44" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="28"/>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
-    </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-    </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
-      <c r="A46" s="27"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="22"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:6" s="1" customFormat="1" ht="9.75" customHeight="1">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" s="1" customFormat="1" ht="9.75" customHeight="1">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:6" s="1" customFormat="1" ht="9.75" customHeight="1">
       <c r="A47" s="4"/>
@@ -2805,14 +2303,14 @@
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="1:5" s="1" customFormat="1" ht="9.75" customHeight="1">
+    <row r="102" spans="1:5" s="1" customFormat="1">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="1:5" s="1" customFormat="1" ht="9.75" customHeight="1">
+    <row r="103" spans="1:5" s="1" customFormat="1">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -2847,35 +2345,21 @@
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="1:5" s="1" customFormat="1">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
+    <row r="108" spans="1:5">
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="1:5" s="1" customFormat="1">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
+    <row r="109" spans="1:5">
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
-    </row>
-    <row r="110" spans="1:5">
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-    </row>
-    <row r="111" spans="1:5">
-      <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
-      <c r="E111" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E35:E46" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E33:E44" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Lower,Higher"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2894,7 +2378,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -2976,7 +2460,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -2986,7 +2470,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -3082,14 +2566,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B59EC22-C81A-4CA2-A5DD-486CD9568D41}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11073B2-9FC2-4B8B-BFC9-54EA03A21348}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3171,7 +2655,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -3181,7 +2665,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -3277,14 +2761,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11073B2-9FC2-4B8B-BFC9-54EA03A21348}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B59EC22-C81A-4CA2-A5DD-486CD9568D41}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3366,7 +2850,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -3376,7 +2860,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -3479,7 +2963,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3561,7 +3045,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -3571,7 +3055,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -3667,14 +3151,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A361A614-467E-4805-85AC-D8607985F816}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40AF2F6-052D-44E3-ABE0-B0ABDF723B15}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3756,7 +3240,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -3766,7 +3250,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -3862,14 +3346,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40AF2F6-052D-44E3-ABE0-B0ABDF723B15}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A361A614-467E-4805-85AC-D8607985F816}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3951,7 +3435,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -3961,7 +3445,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -4064,7 +3548,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4146,7 +3630,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -4156,7 +3640,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -4259,7 +3743,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4341,7 +3825,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -4351,7 +3835,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -4454,7 +3938,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4536,7 +4020,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -4546,7 +4030,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -4649,7 +4133,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4731,7 +4215,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -4741,7 +4225,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -4845,7 +4329,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4927,7 +4411,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -4937,7 +4421,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -5040,7 +4524,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5122,7 +4606,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -5132,7 +4616,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -5235,7 +4719,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5317,7 +4801,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -5327,7 +4811,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -5430,7 +4914,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5512,7 +4996,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -5522,7 +5006,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -5625,7 +5109,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5707,7 +5191,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -5717,7 +5201,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -5820,7 +5304,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5902,7 +5386,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -5912,7 +5396,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -6015,7 +5499,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6097,7 +5581,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -6107,7 +5591,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -6206,11 +5690,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A05267E-DD4E-46E4-9CE0-1BF9CCF95E6E}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6292,7 +5776,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -6302,7 +5786,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -6405,7 +5889,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6487,7 +5971,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -6497,7 +5981,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -6600,7 +6084,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6682,7 +6166,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -6692,7 +6176,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -6795,7 +6279,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6877,7 +6361,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -6887,7 +6371,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -6990,7 +6474,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -7072,7 +6556,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -7082,7 +6566,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -7185,7 +6669,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -7267,7 +6751,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -7277,7 +6761,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -7380,7 +6864,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -7462,7 +6946,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -7472,7 +6956,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -7575,7 +7059,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -7657,7 +7141,7 @@
     <row r="12" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33"/>
     </row>
@@ -7667,7 +7151,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -7763,15 +7247,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x010100339A91ABF6B0E74BBAB45B3A7F6E62EE" ma:contentTypeVersion="" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="6e17012235b26a7a0350590f144b58ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1bbecb3f91f6338ad1582cc9b6c688ac" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7903,6 +7378,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7913,14 +7397,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC26BC8C-8D44-46BE-A39D-C16F3FC5094C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4667855A-3738-433F-9E1F-E8508E1FE58D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7938,6 +7414,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC26BC8C-8D44-46BE-A39D-C16F3FC5094C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9F50EA-511A-47A0-93D9-E0B615D1BBD8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
v0.34 - Fix Korean
</commit_message>
<xml_diff>
--- a/static/Design_Template.xlsx
+++ b/static/Design_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\snowball\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newsistraphael/Pythons/snowball/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DF3126-CD0B-4A2A-A507-3613FE1E7D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7619CD7F-F4D8-5C46-9F58-BCEA7A8F6AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="873" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" tabRatio="873" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,10 @@
   <definedNames>
     <definedName name="_1.매출채권">#REF!</definedName>
     <definedName name="※매출매트릭스">#REF!</definedName>
+    <definedName name="계">#REF!</definedName>
+    <definedName name="ㅁ1">#REF!</definedName>
+    <definedName name="진주원">'[2]4b Consolidated PL'!#REF!</definedName>
+    <definedName name="채권">#REF!</definedName>
     <definedName name="A">'[1]4b Consolidated PL'!#REF!</definedName>
     <definedName name="ddd">#REF!</definedName>
     <definedName name="LYN">'[2]4b Consolidated PL'!#REF!</definedName>
@@ -108,10 +112,6 @@
     <definedName name="Print_Area_MI">#REF!</definedName>
     <definedName name="Question_Type">[4]Values!$B$3:$B$10</definedName>
     <definedName name="SQL_Col">#REF!</definedName>
-    <definedName name="계">#REF!</definedName>
-    <definedName name="ㅁ1">#REF!</definedName>
-    <definedName name="진주원">'[2]4b Consolidated PL'!#REF!</definedName>
-    <definedName name="채권">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1027,6 +1027,20 @@
     <cellStyle name="??&amp;O?&amp;H?_x0008__x000f__x0007_?_x0007__x0001__x0001_" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="??&amp;O?&amp;H?_x0008_??_x0007__x0001__x0001_" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="뒤에 오는 하이퍼링크_금융비용자본화" xfId="5" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="뷭?_BOOKSHIP" xfId="6" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="새귑_롤痰삠悧 " xfId="8" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="새귑[0]_롤痰삠悧 " xfId="7" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="스타일 1" xfId="1" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="지정되지 않음" xfId="9" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="콤마 [0]_  종  합  " xfId="10" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="콤마_  종  합  " xfId="11" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="표준 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="標準_Akia(F）-8" xfId="12" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="표준_Operating_test(1)" xfId="13" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="표준_Sheet1" xfId="14" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
     <cellStyle name="category" xfId="15" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Comma [0]_ SG&amp;A Bridge " xfId="16" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="comma zerodec" xfId="17" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
@@ -1051,20 +1065,6 @@
     <cellStyle name="Output Report Title" xfId="35" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="Percent [2]" xfId="36" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
     <cellStyle name="subhead" xfId="37" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="뒤에 오는 하이퍼링크_금융비용자본화" xfId="5" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="뷭?_BOOKSHIP" xfId="6" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="새귑[0]_롤痰삠悧 " xfId="7" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="새귑_롤痰삠悧 " xfId="8" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="스타일 1" xfId="1" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="지정되지 않음" xfId="9" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="콤마 [0]_  종  합  " xfId="10" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="콤마_  종  합  " xfId="11" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="표준 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="標準_Akia(F）-8" xfId="12" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="표준_Operating_test(1)" xfId="13" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="표준_Sheet1" xfId="14" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1499,13 +1499,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B9" sqref="B9:C10"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.83203125" style="5" customWidth="1"/>
@@ -1532,7 +1532,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A2" s="31" t="s">
         <v>11</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="D2" s="31"/>
       <c r="E2" s="29"/>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
@@ -1554,7 +1554,7 @@
       <c r="D3" s="31"/>
       <c r="E3" s="29"/>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A4" s="31" t="s">
         <v>13</v>
       </c>
@@ -1565,7 +1565,7 @@
       <c r="D4" s="31"/>
       <c r="E4" s="29"/>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A5" s="31" t="s">
         <v>14</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="D5" s="31"/>
       <c r="E5" s="29"/>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A6" s="31" t="s">
         <v>15</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="D6" s="31"/>
       <c r="E6" s="29"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A7" s="31" t="s">
         <v>16</v>
       </c>
@@ -1598,7 +1598,7 @@
       <c r="D7" s="31"/>
       <c r="E7" s="29"/>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A8" s="31" t="s">
         <v>17</v>
       </c>
@@ -1609,7 +1609,7 @@
       <c r="D8" s="31"/>
       <c r="E8" s="29"/>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A9" s="31" t="s">
         <v>18</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="D9" s="31"/>
       <c r="E9" s="29"/>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A10" s="31" t="s">
         <v>19</v>
       </c>
@@ -1631,7 +1631,7 @@
       <c r="D10" s="31"/>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A11" s="31" t="s">
         <v>20</v>
       </c>
@@ -1642,7 +1642,7 @@
       <c r="D11" s="31"/>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A12" s="31" t="s">
         <v>21</v>
       </c>
@@ -1653,7 +1653,7 @@
       <c r="D12" s="31"/>
       <c r="E12" s="29"/>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="13" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A13" s="31" t="s">
         <v>22</v>
       </c>
@@ -1664,7 +1664,7 @@
       <c r="D13" s="31"/>
       <c r="E13" s="29"/>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A14" s="31" t="s">
         <v>23</v>
       </c>
@@ -1675,7 +1675,7 @@
       <c r="D14" s="31"/>
       <c r="E14" s="29"/>
     </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A15" s="31" t="s">
         <v>24</v>
       </c>
@@ -1686,7 +1686,7 @@
       <c r="D15" s="31"/>
       <c r="E15" s="29"/>
     </row>
-    <row r="16" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="16" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A16" s="31" t="s">
         <v>25</v>
       </c>
@@ -1697,7 +1697,7 @@
       <c r="D16" s="31"/>
       <c r="E16" s="29"/>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="17" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A17" s="31" t="s">
         <v>26</v>
       </c>
@@ -1708,7 +1708,7 @@
       <c r="D17" s="31"/>
       <c r="E17" s="29"/>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="18" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A18" s="31" t="s">
         <v>27</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="D18" s="31"/>
       <c r="E18" s="37"/>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A19" s="31" t="s">
         <v>28</v>
       </c>
@@ -1730,7 +1730,7 @@
       <c r="D19" s="31"/>
       <c r="E19" s="29"/>
     </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="20" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A20" s="31" t="s">
         <v>29</v>
       </c>
@@ -1741,7 +1741,7 @@
       <c r="D20" s="31"/>
       <c r="E20" s="29"/>
     </row>
-    <row r="21" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="21" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A21" s="31" t="s">
         <v>30</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="D21" s="31"/>
       <c r="E21" s="29"/>
     </row>
-    <row r="22" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="22" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A22" s="31" t="s">
         <v>31</v>
       </c>
@@ -1763,7 +1763,7 @@
       <c r="D22" s="31"/>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A23" s="31" t="s">
         <v>32</v>
       </c>
@@ -1774,7 +1774,7 @@
       <c r="D23" s="31"/>
       <c r="E23" s="29"/>
     </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A24" s="31" t="s">
         <v>33</v>
       </c>
@@ -1785,7 +1785,7 @@
       <c r="D24" s="31"/>
       <c r="E24" s="29"/>
     </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="25" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A25" s="31" t="s">
         <v>34</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="D25" s="31"/>
       <c r="E25" s="29"/>
     </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A26" s="31" t="s">
         <v>35</v>
       </c>
@@ -1807,7 +1807,7 @@
       <c r="D26" s="31"/>
       <c r="E26" s="29"/>
     </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="27" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A27" s="31" t="s">
         <v>36</v>
       </c>
@@ -1818,7 +1818,7 @@
       <c r="D27" s="31"/>
       <c r="E27" s="29"/>
     </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A28" s="31" t="s">
         <v>37</v>
       </c>
@@ -1829,7 +1829,7 @@
       <c r="D28" s="31"/>
       <c r="E28" s="29"/>
     </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="29" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A29" s="31" t="s">
         <v>38</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="D29" s="31"/>
       <c r="E29" s="29"/>
     </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A30" s="31" t="s">
         <v>39</v>
       </c>
@@ -1851,7 +1851,7 @@
       <c r="D30" s="31"/>
       <c r="E30" s="29"/>
     </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A31" s="31" t="s">
         <v>40</v>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="D31" s="31"/>
       <c r="E31" s="29"/>
     </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" ht="13.5">
+    <row r="32" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A32" s="31" t="s">
         <v>41</v>
       </c>
@@ -1873,14 +1873,14 @@
       <c r="D32" s="31"/>
       <c r="E32" s="29"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A33" s="27"/>
       <c r="B33" s="27"/>
       <c r="C33" s="28"/>
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A34" s="27"/>
       <c r="B34" s="27"/>
       <c r="C34" s="28"/>
@@ -1896,63 +1896,63 @@
       <c r="D35" s="40"/>
       <c r="E35" s="41"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A36" s="27"/>
       <c r="B36" s="27"/>
       <c r="C36" s="28"/>
       <c r="D36" s="29"/>
       <c r="E36" s="29"/>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A37" s="27"/>
       <c r="B37" s="27"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A38" s="27"/>
       <c r="B38" s="27"/>
       <c r="C38" s="28"/>
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A39" s="27"/>
       <c r="B39" s="27"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A40" s="27"/>
       <c r="B40" s="27"/>
       <c r="C40" s="28"/>
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A41" s="27"/>
       <c r="B41" s="27"/>
       <c r="C41" s="28"/>
       <c r="D41" s="29"/>
       <c r="E41" s="29"/>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A42" s="27"/>
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A43" s="27"/>
       <c r="B43" s="27"/>
       <c r="C43" s="28"/>
       <c r="D43" s="29"/>
       <c r="E43" s="29"/>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A44" s="27"/>
       <c r="B44" s="30"/>
       <c r="C44" s="28"/>
@@ -2437,7 +2437,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -2629,10 +2629,10 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -2724,7 +2724,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -2824,10 +2824,10 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -2919,7 +2919,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -3022,7 +3022,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3217,7 +3217,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3309,7 +3309,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -3408,11 +3408,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A361A614-467E-4805-85AC-D8607985F816}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3504,7 +3504,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
@@ -3607,7 +3607,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3802,7 +3802,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -3997,7 +3997,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4192,7 +4192,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4388,7 +4388,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4583,7 +4583,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4778,7 +4778,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -4973,7 +4973,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5168,7 +5168,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5363,7 +5363,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5558,7 +5558,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5753,7 +5753,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -5948,7 +5948,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6143,7 +6143,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6338,7 +6338,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6533,7 +6533,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6728,7 +6728,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -6923,7 +6923,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -7118,7 +7118,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
@@ -7438,21 +7438,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7474,6 +7474,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC26BC8C-8D44-46BE-A39D-C16F3FC5094C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9F50EA-511A-47A0-93D9-E0B615D1BBD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7481,12 +7489,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC26BC8C-8D44-46BE-A39D-C16F3FC5094C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>